<commit_message>
he borrado valores de varias columnas
</commit_message>
<xml_diff>
--- a/metal 2023ConMacro.xlsx
+++ b/metal 2023ConMacro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ficapracticas4\Desktop\PruebaExcel\PruebaExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GitHub\PruebaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8121310-D340-4523-A835-38D2C666BE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF5F8B6-76FE-4311-B62F-7D30A682689C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="601" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23058,8 +23058,8 @@
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23318,276 +23318,132 @@
         <v>2892.010000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17">
-        <v>23539.700000000004</v>
-      </c>
-      <c r="D17">
-        <v>13.466647597254006</v>
-      </c>
-      <c r="E17">
-        <v>8419.7000000000044</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>22957.599999999999</v>
-      </c>
-      <c r="D18">
-        <v>13.007138810198299</v>
-      </c>
-      <c r="E18">
-        <v>7837.5999999999985</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
-        <v>21707.66</v>
-      </c>
-      <c r="D19">
-        <v>12.418569794050343</v>
-      </c>
-      <c r="E19">
-        <v>6587.66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C20">
-        <v>16945.88</v>
-      </c>
-      <c r="D20">
-        <v>9.2803285870755747</v>
-      </c>
-      <c r="E20">
-        <v>1825.880000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="C21">
-        <v>20509.55</v>
-      </c>
-      <c r="D21">
-        <v>11.613561721404302</v>
-      </c>
-      <c r="E21">
-        <v>5389.5499999999993</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22">
-        <v>28154.5334</v>
-      </c>
-      <c r="D22">
-        <v>16.015092946530149</v>
-      </c>
-      <c r="E22">
-        <v>13034.5334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23">
-        <v>24071.1</v>
-      </c>
-      <c r="D23">
-        <v>13.739212328767122</v>
-      </c>
-      <c r="E23">
-        <v>8951.0999999999985</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C24">
-        <v>17273.099999999999</v>
-      </c>
-      <c r="D24">
-        <v>9.7368094701240135</v>
-      </c>
-      <c r="E24">
-        <v>2153.0999999999985</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
-      <c r="C25">
-        <v>23477.41</v>
-      </c>
-      <c r="D25">
-        <v>13.477273249138921</v>
-      </c>
-      <c r="E25">
-        <v>8357.41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26">
-        <v>20510.499999999996</v>
-      </c>
-      <c r="D26">
-        <v>11.653693181818181</v>
-      </c>
-      <c r="E26">
-        <v>5390.4999999999964</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="C27">
-        <v>18331.04</v>
-      </c>
-      <c r="D27">
-        <v>10.415363636363637</v>
-      </c>
-      <c r="E27">
-        <v>3211.0400000000009</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
-      <c r="C28">
-        <v>28650.516</v>
-      </c>
-      <c r="D28">
-        <v>17.033600475624258</v>
-      </c>
-      <c r="E28">
-        <v>13530.516</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C29">
-        <v>24929.45</v>
-      </c>
-      <c r="D29">
-        <v>14.343757192174914</v>
-      </c>
-      <c r="E29">
-        <v>9809.4500000000007</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="C30">
-        <v>23719.15</v>
-      </c>
-      <c r="D30">
-        <v>13.663104838709678</v>
-      </c>
-      <c r="E30">
-        <v>8599.1500000000015</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="C31">
-        <v>20423.09</v>
-      </c>
-      <c r="D31">
-        <v>11.60402840909091</v>
-      </c>
-      <c r="E31">
-        <v>5303.09</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
-      </c>
-      <c r="C32">
-        <v>18912.419999999998</v>
-      </c>
-      <c r="D32">
-        <v>10.709184597961494</v>
-      </c>
-      <c r="E32">
-        <v>3792.4199999999983</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -23597,15 +23453,6 @@
       <c r="B33" t="s">
         <v>6</v>
       </c>
-      <c r="C33">
-        <v>22023.960000000003</v>
-      </c>
-      <c r="D33">
-        <v>12.570753424657536</v>
-      </c>
-      <c r="E33">
-        <v>6903.9600000000028</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -23614,15 +23461,6 @@
       <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C34">
-        <v>18651.96</v>
-      </c>
-      <c r="D34">
-        <v>10.579671015314803</v>
-      </c>
-      <c r="E34">
-        <v>3531.9599999999991</v>
-      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -23631,15 +23469,6 @@
       <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="C35">
-        <v>21008.720000000001</v>
-      </c>
-      <c r="D35">
-        <v>11.815928008998876</v>
-      </c>
-      <c r="E35">
-        <v>5888.7200000000012</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -23648,15 +23477,6 @@
       <c r="B36" t="s">
         <v>6</v>
       </c>
-      <c r="C36">
-        <v>20574.169999999998</v>
-      </c>
-      <c r="D36">
-        <v>11.663361678004534</v>
-      </c>
-      <c r="E36">
-        <v>5454.1699999999983</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -23664,15 +23484,6 @@
       </c>
       <c r="B37" t="s">
         <v>6</v>
-      </c>
-      <c r="C37">
-        <v>21560.28</v>
-      </c>
-      <c r="D37">
-        <v>12.278063781321183</v>
-      </c>
-      <c r="E37">
-        <v>6440.2799999999988</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>